<commit_message>
attempts to plot predicted values
</commit_message>
<xml_diff>
--- a/Seagrass_2017/Eelgrass_structure_MS_results/Models_top3.xlsx
+++ b/Seagrass_2017/Eelgrass_structure_MS_results/Models_top3.xlsx
@@ -502,7 +502,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="4">
-        <v>24.31</v>
+        <v>64.31</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>